<commit_message>
started analysis of novelty and surprise from vertColum and CervCancer Dataset
</commit_message>
<xml_diff>
--- a/results_analysis/spark_vertebralColum_02_hold2.xlsx
+++ b/results_analysis/spark_vertebralColum_02_hold2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4513E232-1088-4735-9C90-109482CC5DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0358D08-6418-4180-902E-13F3CBC045DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_best" sheetId="11" r:id="rId1"/>
@@ -695,24 +695,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -789,6 +771,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1074,7 +1074,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,19 +1092,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1158,10 +1158,10 @@
       <c r="E5" s="12">
         <v>0.79411764705882404</v>
       </c>
-      <c r="F5" s="64">
+      <c r="F5" s="58">
         <v>0.870588235294118</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="58">
         <v>0.84117647058823497</v>
       </c>
       <c r="H5" s="12">
@@ -1170,10 +1170,10 @@
       <c r="I5" s="12">
         <v>0.78235294117647103</v>
       </c>
-      <c r="J5" s="64">
+      <c r="J5" s="58">
         <v>0.84117647058823497</v>
       </c>
-      <c r="K5" s="65">
+      <c r="K5" s="59">
         <v>0.84705882352941197</v>
       </c>
     </row>
@@ -1185,13 +1185,13 @@
       <c r="D6" s="48">
         <v>0.81764705882352895</v>
       </c>
-      <c r="E6" s="66">
+      <c r="E6" s="60">
         <v>0.86470588235294099</v>
       </c>
       <c r="F6" s="13">
         <v>0.72941176470588198</v>
       </c>
-      <c r="G6" s="66">
+      <c r="G6" s="60">
         <v>0.82941176470588196</v>
       </c>
       <c r="H6" s="13">
@@ -1200,7 +1200,7 @@
       <c r="I6" s="13">
         <v>0.81764705882352895</v>
       </c>
-      <c r="J6" s="66">
+      <c r="J6" s="60">
         <v>0.870588235294118</v>
       </c>
       <c r="K6" s="15">
@@ -1215,7 +1215,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="67">
+      <c r="D7" s="61">
         <v>0.78823529411764703</v>
       </c>
       <c r="E7" s="13">
@@ -1224,7 +1224,7 @@
       <c r="F7" s="13">
         <v>0.71764705882352897</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="60">
         <v>0.78823529411764703</v>
       </c>
       <c r="H7" s="13">
@@ -1233,10 +1233,10 @@
       <c r="I7" s="13">
         <v>0.752941176470588</v>
       </c>
-      <c r="J7" s="66">
+      <c r="J7" s="60">
         <v>0.83529411764705896</v>
       </c>
-      <c r="K7" s="70">
+      <c r="K7" s="64">
         <v>0.85294117647058798</v>
       </c>
     </row>
@@ -1252,7 +1252,7 @@
       <c r="E8" s="14">
         <v>0.82941176470588196</v>
       </c>
-      <c r="F8" s="68">
+      <c r="F8" s="62">
         <v>0.870588235294118</v>
       </c>
       <c r="G8" s="14">
@@ -1264,10 +1264,10 @@
       <c r="I8" s="14">
         <v>0.8</v>
       </c>
-      <c r="J8" s="68">
+      <c r="J8" s="62">
         <v>0.876470588235294</v>
       </c>
-      <c r="K8" s="71">
+      <c r="K8" s="65">
         <v>0.84705882352941197</v>
       </c>
     </row>
@@ -1284,13 +1284,13 @@
       <c r="D9" s="51">
         <v>0.78823529411764703</v>
       </c>
-      <c r="E9" s="69">
+      <c r="E9" s="63">
         <v>0.82941176470588196</v>
       </c>
       <c r="F9" s="52">
         <v>0.79411764705882404</v>
       </c>
-      <c r="G9" s="69">
+      <c r="G9" s="63">
         <v>0.82941176470588196</v>
       </c>
       <c r="H9" s="52">
@@ -1299,7 +1299,7 @@
       <c r="I9" s="52">
         <v>0.82352941176470595</v>
       </c>
-      <c r="J9" s="69">
+      <c r="J9" s="63">
         <v>0.84705882352941197</v>
       </c>
       <c r="K9" s="53">
@@ -1314,16 +1314,16 @@
       <c r="D10" s="48">
         <v>0.82941176470588196</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="60">
         <v>0.870588235294118</v>
       </c>
       <c r="F10" s="13">
         <v>0.82941176470588196</v>
       </c>
-      <c r="G10" s="66">
+      <c r="G10" s="60">
         <v>0.85294117647058798</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="60">
         <v>0.870588235294118</v>
       </c>
       <c r="I10" s="13">
@@ -1344,7 +1344,7 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="67">
+      <c r="D11" s="61">
         <v>0.85294117647058798</v>
       </c>
       <c r="E11" s="13">
@@ -1356,10 +1356,10 @@
       <c r="G11" s="13">
         <v>0.78235294117647103</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="60">
         <v>0.81764705882352895</v>
       </c>
-      <c r="I11" s="66">
+      <c r="I11" s="60">
         <v>0.84705882352941197</v>
       </c>
       <c r="J11" s="13">
@@ -1378,7 +1378,7 @@
       <c r="D12" s="49">
         <v>0.77058823529411802</v>
       </c>
-      <c r="E12" s="68">
+      <c r="E12" s="62">
         <v>0.870588235294118</v>
       </c>
       <c r="F12" s="14">
@@ -1393,10 +1393,10 @@
       <c r="I12" s="14">
         <v>0.7</v>
       </c>
-      <c r="J12" s="68">
+      <c r="J12" s="62">
         <v>0.84117647058823497</v>
       </c>
-      <c r="K12" s="71">
+      <c r="K12" s="65">
         <v>0.85882352941176499</v>
       </c>
     </row>
@@ -1416,19 +1416,19 @@
       <c r="E13" s="52">
         <v>0.75882352941176501</v>
       </c>
-      <c r="F13" s="69">
+      <c r="F13" s="63">
         <v>0.8</v>
       </c>
-      <c r="G13" s="69">
+      <c r="G13" s="63">
         <v>0.79411764705882404</v>
       </c>
-      <c r="H13" s="69">
+      <c r="H13" s="63">
         <v>0.79411764705882404</v>
       </c>
       <c r="I13" s="52">
         <v>0.78823529411764703</v>
       </c>
-      <c r="J13" s="69">
+      <c r="J13" s="63">
         <v>0.876470588235294</v>
       </c>
       <c r="K13" s="53">
@@ -1440,7 +1440,7 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="67">
+      <c r="D14" s="61">
         <v>0.86470588235294099</v>
       </c>
       <c r="E14" s="13">
@@ -1455,10 +1455,10 @@
       <c r="H14" s="13">
         <v>0.81764705882352895</v>
       </c>
-      <c r="I14" s="66">
+      <c r="I14" s="60">
         <v>0.88235294117647101</v>
       </c>
-      <c r="J14" s="66">
+      <c r="J14" s="60">
         <v>0.85294117647058798</v>
       </c>
       <c r="K14" s="15">
@@ -1473,7 +1473,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="67">
+      <c r="D15" s="61">
         <v>0.84117647058823497</v>
       </c>
       <c r="E15" s="13">
@@ -1485,7 +1485,7 @@
       <c r="G15" s="13">
         <v>0.72352941176470598</v>
       </c>
-      <c r="H15" s="66">
+      <c r="H15" s="60">
         <v>0.84117647058823497</v>
       </c>
       <c r="I15" s="13">
@@ -1494,7 +1494,7 @@
       <c r="J15" s="13">
         <v>0.6</v>
       </c>
-      <c r="K15" s="70">
+      <c r="K15" s="64">
         <v>0.82941176470588196</v>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       <c r="D16" s="49">
         <v>0.74117647058823499</v>
       </c>
-      <c r="E16" s="68">
+      <c r="E16" s="62">
         <v>0.77058823529411802</v>
       </c>
       <c r="F16" s="14">
@@ -1516,10 +1516,10 @@
       <c r="G16" s="14">
         <v>0.65882352941176503</v>
       </c>
-      <c r="H16" s="68">
+      <c r="H16" s="62">
         <v>0.75882352941176501</v>
       </c>
-      <c r="I16" s="68">
+      <c r="I16" s="62">
         <v>0.752941176470588</v>
       </c>
       <c r="J16" s="14">
@@ -1542,10 +1542,10 @@
       <c r="D17" s="51">
         <v>0.81764705882352895</v>
       </c>
-      <c r="E17" s="69">
+      <c r="E17" s="63">
         <v>0.84117647058823497</v>
       </c>
-      <c r="F17" s="69">
+      <c r="F17" s="63">
         <v>0.84705882352941197</v>
       </c>
       <c r="G17" s="52">
@@ -1554,7 +1554,7 @@
       <c r="H17" s="52">
         <v>0.75882352941176501</v>
       </c>
-      <c r="I17" s="69">
+      <c r="I17" s="63">
         <v>0.84117647058823497</v>
       </c>
       <c r="J17" s="52">
@@ -1569,19 +1569,19 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="67">
+      <c r="D18" s="61">
         <v>0.82352941176470595</v>
       </c>
       <c r="E18" s="13">
         <v>0.81176470588235305</v>
       </c>
-      <c r="F18" s="66">
+      <c r="F18" s="60">
         <v>0.84117647058823497</v>
       </c>
       <c r="G18" s="13">
         <v>0.80588235294117705</v>
       </c>
-      <c r="H18" s="66">
+      <c r="H18" s="60">
         <v>0.85294117647058798</v>
       </c>
       <c r="I18" s="13">
@@ -1608,7 +1608,7 @@
       <c r="E19" s="13">
         <v>0.81176470588235305</v>
       </c>
-      <c r="F19" s="66">
+      <c r="F19" s="60">
         <v>0.82352941176470595</v>
       </c>
       <c r="G19" s="13">
@@ -1620,10 +1620,10 @@
       <c r="I19" s="13">
         <v>0.747058823529412</v>
       </c>
-      <c r="J19" s="66">
+      <c r="J19" s="60">
         <v>0.82352941176470595</v>
       </c>
-      <c r="K19" s="70">
+      <c r="K19" s="64">
         <v>0.82352941176470595</v>
       </c>
     </row>
@@ -1636,7 +1636,7 @@
       <c r="D20" s="49">
         <v>0.8</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="62">
         <v>0.85294117647058798</v>
       </c>
       <c r="F20" s="14">
@@ -1645,13 +1645,13 @@
       <c r="G20" s="14">
         <v>0.78823529411764703</v>
       </c>
-      <c r="H20" s="68">
+      <c r="H20" s="62">
         <v>0.84705882352941197</v>
       </c>
       <c r="I20" s="14">
         <v>0.71176470588235297</v>
       </c>
-      <c r="J20" s="68">
+      <c r="J20" s="62">
         <v>0.84705882352941197</v>
       </c>
       <c r="K20" s="50">
@@ -2002,7 +2002,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,19 +2013,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -2605,7 +2605,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2616,19 +2616,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3207,8 +3207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" activeCellId="5" sqref="D15 H15 I15 D16 F16 I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3226,19 +3226,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3292,10 +3292,10 @@
       <c r="E5" s="12">
         <v>0.68882352941176495</v>
       </c>
-      <c r="F5" s="64">
+      <c r="F5" s="58">
         <v>0.73058823529411798</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="58">
         <v>0.71705882352941197</v>
       </c>
       <c r="H5" s="12">
@@ -3307,7 +3307,7 @@
       <c r="J5" s="12">
         <v>0.69470588235294095</v>
       </c>
-      <c r="K5" s="65">
+      <c r="K5" s="59">
         <v>0.71294117647058797</v>
       </c>
     </row>
@@ -3319,19 +3319,19 @@
       <c r="D6" s="48">
         <v>0.65764705882353003</v>
       </c>
-      <c r="E6" s="66">
+      <c r="E6" s="60">
         <v>0.746470588235294</v>
       </c>
       <c r="F6" s="13">
         <v>0.64294117647058802</v>
       </c>
-      <c r="G6" s="66">
+      <c r="G6" s="60">
         <v>0.73705882352941199</v>
       </c>
       <c r="H6" s="13">
         <v>0.7</v>
       </c>
-      <c r="I6" s="66">
+      <c r="I6" s="60">
         <v>0.74235294117647099</v>
       </c>
       <c r="J6" s="13">
@@ -3349,7 +3349,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="67">
+      <c r="D7" s="61">
         <v>0.70058823529411796</v>
       </c>
       <c r="E7" s="13">
@@ -3361,13 +3361,13 @@
       <c r="G7" s="13">
         <v>0.64647058823529402</v>
       </c>
-      <c r="H7" s="66">
+      <c r="H7" s="60">
         <v>0.68529411764705905</v>
       </c>
       <c r="I7" s="13">
         <v>0.47058823529411797</v>
       </c>
-      <c r="J7" s="66">
+      <c r="J7" s="60">
         <v>0.71823529411764697</v>
       </c>
       <c r="K7" s="15">
@@ -3383,10 +3383,10 @@
       <c r="D8" s="49">
         <v>0.68352941176470605</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="62">
         <v>0.72470588235294098</v>
       </c>
-      <c r="F8" s="68">
+      <c r="F8" s="62">
         <v>0.69529411764705895</v>
       </c>
       <c r="G8" s="14">
@@ -3398,7 +3398,7 @@
       <c r="I8" s="14">
         <v>0.55176470588235305</v>
       </c>
-      <c r="J8" s="68">
+      <c r="J8" s="62">
         <v>0.69941176470588196</v>
       </c>
       <c r="K8" s="50">
@@ -3424,16 +3424,16 @@
       <c r="F9" s="52">
         <v>0.70235294117647096</v>
       </c>
-      <c r="G9" s="69">
+      <c r="G9" s="63">
         <v>0.73</v>
       </c>
-      <c r="H9" s="69">
+      <c r="H9" s="63">
         <v>0.73705882352941199</v>
       </c>
       <c r="I9" s="52">
         <v>0.5</v>
       </c>
-      <c r="J9" s="69">
+      <c r="J9" s="63">
         <v>0.72588235294117598</v>
       </c>
       <c r="K9" s="53">
@@ -3445,7 +3445,7 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="67">
+      <c r="D10" s="61">
         <v>0.754705882352941</v>
       </c>
       <c r="E10" s="13">
@@ -3457,7 +3457,7 @@
       <c r="G10" s="13">
         <v>0.73882352941176499</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="60">
         <v>0.79058823529411804</v>
       </c>
       <c r="I10" s="13">
@@ -3466,7 +3466,7 @@
       <c r="J10" s="13">
         <v>0.70588235294117596</v>
       </c>
-      <c r="K10" s="70">
+      <c r="K10" s="64">
         <v>0.75823529411764701</v>
       </c>
     </row>
@@ -3478,7 +3478,7 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="67">
+      <c r="D11" s="61">
         <v>0.68117647058823505</v>
       </c>
       <c r="E11" s="13">
@@ -3490,13 +3490,13 @@
       <c r="G11" s="13">
         <v>0.69411764705882395</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="60">
         <v>0.68647058823529405</v>
       </c>
       <c r="I11" s="13">
         <v>0.64176470588235301</v>
       </c>
-      <c r="J11" s="66">
+      <c r="J11" s="60">
         <v>0.72058823529411797</v>
       </c>
       <c r="K11" s="15">
@@ -3512,7 +3512,7 @@
       <c r="D12" s="49">
         <v>0.69</v>
       </c>
-      <c r="E12" s="68">
+      <c r="E12" s="62">
         <v>0.75705882352941201</v>
       </c>
       <c r="F12" s="14">
@@ -3521,7 +3521,7 @@
       <c r="G12" s="14">
         <v>0.72588235294117598</v>
       </c>
-      <c r="H12" s="68">
+      <c r="H12" s="62">
         <v>0.754117647058824</v>
       </c>
       <c r="I12" s="14">
@@ -3530,7 +3530,7 @@
       <c r="J12" s="14">
         <v>0.68470588235294105</v>
       </c>
-      <c r="K12" s="71">
+      <c r="K12" s="65">
         <v>0.76705882352941201</v>
       </c>
     </row>
@@ -3550,10 +3550,10 @@
       <c r="E13" s="52">
         <v>0.68470588235294105</v>
       </c>
-      <c r="F13" s="69">
+      <c r="F13" s="63">
         <v>0.72235294117647098</v>
       </c>
-      <c r="G13" s="69">
+      <c r="G13" s="63">
         <v>0.72529411764705898</v>
       </c>
       <c r="H13" s="52">
@@ -3562,7 +3562,7 @@
       <c r="I13" s="52">
         <v>0.68764705882353006</v>
       </c>
-      <c r="J13" s="69">
+      <c r="J13" s="63">
         <v>0.73176470588235298</v>
       </c>
       <c r="K13" s="53">
@@ -3580,7 +3580,7 @@
       <c r="E14" s="13">
         <v>0.73352941176470599</v>
       </c>
-      <c r="F14" s="66">
+      <c r="F14" s="60">
         <v>0.76176470588235301</v>
       </c>
       <c r="G14" s="13">
@@ -3589,10 +3589,10 @@
       <c r="H14" s="13">
         <v>0.69411764705882395</v>
       </c>
-      <c r="I14" s="66">
+      <c r="I14" s="60">
         <v>0.77235294117647102</v>
       </c>
-      <c r="J14" s="66">
+      <c r="J14" s="60">
         <v>0.75588235294117601</v>
       </c>
       <c r="K14" s="15">
@@ -3607,7 +3607,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="67">
+      <c r="D15" s="61">
         <v>0.625882352941176</v>
       </c>
       <c r="E15" s="13">
@@ -3619,10 +3619,10 @@
       <c r="G15" s="13">
         <v>0.35823529411764699</v>
       </c>
-      <c r="H15" s="66">
+      <c r="H15" s="60">
         <v>0.55529411764705905</v>
       </c>
-      <c r="I15" s="66">
+      <c r="I15" s="60">
         <v>0.53529411764705903</v>
       </c>
       <c r="J15" s="13">
@@ -3638,13 +3638,13 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="89">
+      <c r="D16" s="83">
         <v>0.54058823529411804</v>
       </c>
       <c r="E16" s="14">
         <v>0.40647058823529397</v>
       </c>
-      <c r="F16" s="68">
+      <c r="F16" s="62">
         <v>0.52882352941176503</v>
       </c>
       <c r="G16" s="14">
@@ -3653,7 +3653,7 @@
       <c r="H16" s="14">
         <v>0.47235294117647098</v>
       </c>
-      <c r="I16" s="68">
+      <c r="I16" s="62">
         <v>0.53647058823529403</v>
       </c>
       <c r="J16" s="14">
@@ -3673,10 +3673,10 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="73">
+      <c r="D17" s="67">
         <v>0.73411764705882399</v>
       </c>
-      <c r="E17" s="69">
+      <c r="E17" s="63">
         <v>0.77235294117647102</v>
       </c>
       <c r="F17" s="52">
@@ -3694,7 +3694,7 @@
       <c r="J17" s="52">
         <v>0.65352941176470603</v>
       </c>
-      <c r="K17" s="72">
+      <c r="K17" s="66">
         <v>0.74294117647058799</v>
       </c>
     </row>
@@ -3703,7 +3703,7 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="67">
+      <c r="D18" s="61">
         <v>0.77529411764705902</v>
       </c>
       <c r="E18" s="13">
@@ -3715,7 +3715,7 @@
       <c r="G18" s="13">
         <v>0.68647058823529405</v>
       </c>
-      <c r="H18" s="66">
+      <c r="H18" s="60">
         <v>0.73058823529411798</v>
       </c>
       <c r="I18" s="13">
@@ -3724,7 +3724,7 @@
       <c r="J18" s="13">
         <v>0.70235294117647096</v>
       </c>
-      <c r="K18" s="70">
+      <c r="K18" s="64">
         <v>0.73235294117647098</v>
       </c>
     </row>
@@ -3736,13 +3736,13 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="67">
+      <c r="D19" s="61">
         <v>0.71470588235294097</v>
       </c>
       <c r="E19" s="13">
         <v>0.65705882352941203</v>
       </c>
-      <c r="F19" s="66">
+      <c r="F19" s="60">
         <v>0.72352941176470598</v>
       </c>
       <c r="G19" s="13">
@@ -3754,7 +3754,7 @@
       <c r="I19" s="13">
         <v>0.63764705882352901</v>
       </c>
-      <c r="J19" s="66">
+      <c r="J19" s="60">
         <v>0.73235294117647098</v>
       </c>
       <c r="K19" s="15">
@@ -3770,7 +3770,7 @@
       <c r="D20" s="49">
         <v>0.66058823529411803</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="62">
         <v>0.71705882352941197</v>
       </c>
       <c r="F20" s="14">
@@ -3785,10 +3785,10 @@
       <c r="I20" s="14">
         <v>0.63411764705882401</v>
       </c>
-      <c r="J20" s="68">
+      <c r="J20" s="62">
         <v>0.70882352941176496</v>
       </c>
-      <c r="K20" s="71">
+      <c r="K20" s="65">
         <v>0.70294117647058796</v>
       </c>
     </row>
@@ -4135,8 +4135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E17B74-8A06-473F-B1B4-0C752BEBC712}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" activeCellId="5" sqref="D15 I15 H15 K16 D16 I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4154,19 +4154,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4220,16 +4220,16 @@
       <c r="E5" s="13">
         <v>0.67941176470588205</v>
       </c>
-      <c r="F5" s="66">
+      <c r="F5" s="60">
         <v>0.76764705882352902</v>
       </c>
       <c r="G5" s="13">
         <v>0.72941176470588198</v>
       </c>
-      <c r="H5" s="66">
+      <c r="H5" s="60">
         <v>0.71176470588235297</v>
       </c>
-      <c r="I5" s="66">
+      <c r="I5" s="60">
         <v>0.72058823529411797</v>
       </c>
       <c r="J5" s="13">
@@ -4247,19 +4247,19 @@
       <c r="D6" s="13">
         <v>0.67941176470588205</v>
       </c>
-      <c r="E6" s="66">
+      <c r="E6" s="60">
         <v>0.73529411764705899</v>
       </c>
       <c r="F6" s="13">
         <v>0.63823529411764701</v>
       </c>
-      <c r="G6" s="66">
+      <c r="G6" s="60">
         <v>0.73235294117647098</v>
       </c>
       <c r="H6" s="13">
         <v>0.70588235294117596</v>
       </c>
-      <c r="I6" s="66">
+      <c r="I6" s="60">
         <v>0.75588235294117601</v>
       </c>
       <c r="J6" s="13">
@@ -4277,7 +4277,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="66">
+      <c r="D7" s="60">
         <v>0.70588235294117596</v>
       </c>
       <c r="E7" s="13">
@@ -4286,7 +4286,7 @@
       <c r="F7" s="13">
         <v>0.67058823529411804</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="60">
         <v>0.70294117647058796</v>
       </c>
       <c r="H7" s="13">
@@ -4295,7 +4295,7 @@
       <c r="I7" s="13">
         <v>0.50882352941176501</v>
       </c>
-      <c r="J7" s="66">
+      <c r="J7" s="60">
         <v>0.72647058823529398</v>
       </c>
       <c r="K7" s="13">
@@ -4308,13 +4308,13 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="66">
+      <c r="D8" s="60">
         <v>0.7</v>
       </c>
-      <c r="E8" s="66">
+      <c r="E8" s="60">
         <v>0.75588235294117601</v>
       </c>
-      <c r="F8" s="66">
+      <c r="F8" s="60">
         <v>0.70588235294117696</v>
       </c>
       <c r="G8" s="13">
@@ -4352,16 +4352,16 @@
       <c r="F9" s="13">
         <v>0.70882352941176496</v>
       </c>
-      <c r="G9" s="66">
+      <c r="G9" s="60">
         <v>0.74117647058823499</v>
       </c>
-      <c r="H9" s="66">
+      <c r="H9" s="60">
         <v>0.74117647058823499</v>
       </c>
       <c r="I9" s="13">
         <v>0.5</v>
       </c>
-      <c r="J9" s="66">
+      <c r="J9" s="60">
         <v>0.74411764705882399</v>
       </c>
       <c r="K9" s="13">
@@ -4373,7 +4373,7 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="66">
+      <c r="D10" s="60">
         <v>0.75882352941176501</v>
       </c>
       <c r="E10" s="13">
@@ -4385,7 +4385,7 @@
       <c r="G10" s="13">
         <v>0.73823529411764699</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="60">
         <v>0.80294117647058805</v>
       </c>
       <c r="I10" s="13">
@@ -4394,7 +4394,7 @@
       <c r="J10" s="13">
         <v>0.72352941176470598</v>
       </c>
-      <c r="K10" s="66">
+      <c r="K10" s="60">
         <v>0.76764705882352902</v>
       </c>
     </row>
@@ -4409,13 +4409,13 @@
       <c r="D11" s="13">
         <v>0.68823529411764695</v>
       </c>
-      <c r="E11" s="66">
+      <c r="E11" s="60">
         <v>0.70588235294117696</v>
       </c>
       <c r="F11" s="13">
         <v>0.67352941176470604</v>
       </c>
-      <c r="G11" s="66">
+      <c r="G11" s="60">
         <v>0.752941176470588</v>
       </c>
       <c r="H11" s="13">
@@ -4424,7 +4424,7 @@
       <c r="I11" s="13">
         <v>0.66470588235294104</v>
       </c>
-      <c r="J11" s="66">
+      <c r="J11" s="60">
         <v>0.71764705882352897</v>
       </c>
       <c r="K11" s="13">
@@ -4440,7 +4440,7 @@
       <c r="D12" s="13">
         <v>0.72058823529411797</v>
       </c>
-      <c r="E12" s="66">
+      <c r="E12" s="60">
         <v>0.75</v>
       </c>
       <c r="F12" s="13">
@@ -4449,7 +4449,7 @@
       <c r="G12" s="13">
         <v>0.73529411764705899</v>
       </c>
-      <c r="H12" s="66">
+      <c r="H12" s="60">
         <v>0.76176470588235301</v>
       </c>
       <c r="I12" s="13">
@@ -4458,7 +4458,7 @@
       <c r="J12" s="13">
         <v>0.67352941176470604</v>
       </c>
-      <c r="K12" s="66">
+      <c r="K12" s="60">
         <v>0.78235294117647103</v>
       </c>
     </row>
@@ -4478,19 +4478,19 @@
       <c r="E13" s="13">
         <v>0.7</v>
       </c>
-      <c r="F13" s="66">
+      <c r="F13" s="60">
         <v>0.72058823529411797</v>
       </c>
-      <c r="G13" s="66">
+      <c r="G13" s="60">
         <v>0.73529411764705899</v>
       </c>
-      <c r="H13" s="66">
+      <c r="H13" s="60">
         <v>0.71176470588235297</v>
       </c>
-      <c r="I13" s="66">
+      <c r="I13" s="60">
         <v>0.72352941176470598</v>
       </c>
-      <c r="J13" s="66">
+      <c r="J13" s="60">
         <v>0.72058823529411797</v>
       </c>
       <c r="K13" s="13">
@@ -4508,7 +4508,7 @@
       <c r="E14" s="13">
         <v>0.73823529411764699</v>
       </c>
-      <c r="F14" s="66">
+      <c r="F14" s="60">
         <v>0.77647058823529402</v>
       </c>
       <c r="G14" s="13">
@@ -4517,10 +4517,10 @@
       <c r="H14" s="13">
         <v>0.7</v>
       </c>
-      <c r="I14" s="66">
+      <c r="I14" s="60">
         <v>0.75882352941176501</v>
       </c>
-      <c r="J14" s="66">
+      <c r="J14" s="60">
         <v>0.752941176470588</v>
       </c>
       <c r="K14" s="13">
@@ -4535,7 +4535,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="66">
+      <c r="D15" s="60">
         <v>0.66470588235294104</v>
       </c>
       <c r="E15" s="13">
@@ -4547,10 +4547,10 @@
       <c r="G15" s="13">
         <v>0.34705882352941197</v>
       </c>
-      <c r="H15" s="66">
+      <c r="H15" s="60">
         <v>0.58529411764705896</v>
       </c>
-      <c r="I15" s="66">
+      <c r="I15" s="60">
         <v>0.52058823529411802</v>
       </c>
       <c r="J15" s="13">
@@ -4566,7 +4566,7 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="66">
+      <c r="D16" s="60">
         <v>0.53235294117647103</v>
       </c>
       <c r="E16" s="13">
@@ -4581,13 +4581,13 @@
       <c r="H16" s="13">
         <v>0.46176470588235302</v>
       </c>
-      <c r="I16" s="66">
+      <c r="I16" s="60">
         <v>0.52352941176470602</v>
       </c>
       <c r="J16" s="13">
         <v>0.36176470588235299</v>
       </c>
-      <c r="K16" s="66">
+      <c r="K16" s="60">
         <v>0.56470588235294095</v>
       </c>
     </row>
@@ -4604,10 +4604,10 @@
       <c r="D17" s="13">
         <v>0.72647058823529398</v>
       </c>
-      <c r="E17" s="66">
+      <c r="E17" s="60">
         <v>0.76176470588235301</v>
       </c>
-      <c r="F17" s="66">
+      <c r="F17" s="60">
         <v>0.76470588235294101</v>
       </c>
       <c r="G17" s="13">
@@ -4622,7 +4622,7 @@
       <c r="J17" s="13">
         <v>0.68235294117647105</v>
       </c>
-      <c r="K17" s="66">
+      <c r="K17" s="60">
         <v>0.75588235294117601</v>
       </c>
     </row>
@@ -4631,10 +4631,10 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="66">
+      <c r="D18" s="60">
         <v>0.78823529411764703</v>
       </c>
-      <c r="E18" s="66">
+      <c r="E18" s="60">
         <v>0.77058823529411802</v>
       </c>
       <c r="F18" s="13">
@@ -4652,7 +4652,7 @@
       <c r="J18" s="13">
         <v>0.71764705882352897</v>
       </c>
-      <c r="K18" s="66">
+      <c r="K18" s="60">
         <v>0.75</v>
       </c>
     </row>
@@ -4664,13 +4664,13 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="66">
+      <c r="D19" s="60">
         <v>0.73235294117647098</v>
       </c>
       <c r="E19" s="13">
         <v>0.64411764705882402</v>
       </c>
-      <c r="F19" s="66">
+      <c r="F19" s="60">
         <v>0.71470588235294097</v>
       </c>
       <c r="G19" s="13">
@@ -4682,7 +4682,7 @@
       <c r="I19" s="13">
         <v>0.66176470588235303</v>
       </c>
-      <c r="J19" s="66">
+      <c r="J19" s="60">
         <v>0.73529411764705899</v>
       </c>
       <c r="K19" s="13">
@@ -4701,13 +4701,13 @@
       <c r="E20" s="13">
         <v>0.7</v>
       </c>
-      <c r="F20" s="66">
+      <c r="F20" s="60">
         <v>0.70294117647058796</v>
       </c>
-      <c r="G20" s="66">
+      <c r="G20" s="60">
         <v>0.70294117647058796</v>
       </c>
-      <c r="H20" s="66">
+      <c r="H20" s="60">
         <v>0.73235294117647098</v>
       </c>
       <c r="I20" s="13">
@@ -4716,7 +4716,7 @@
       <c r="J20" s="13">
         <v>0.67941176470588205</v>
       </c>
-      <c r="K20" s="66">
+      <c r="K20" s="60">
         <v>0.71470588235294097</v>
       </c>
     </row>
@@ -4906,7 +4906,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4924,19 +4924,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4984,28 +4984,28 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="74">
+      <c r="D5" s="68">
         <v>9</v>
       </c>
-      <c r="E5" s="75">
+      <c r="E5" s="69">
         <v>18</v>
       </c>
-      <c r="F5" s="76">
+      <c r="F5" s="70">
         <v>6</v>
       </c>
-      <c r="G5" s="76">
+      <c r="G5" s="70">
         <v>8</v>
       </c>
-      <c r="H5" s="75">
+      <c r="H5" s="69">
         <v>23</v>
       </c>
-      <c r="I5" s="75">
+      <c r="I5" s="69">
         <v>112</v>
       </c>
-      <c r="J5" s="76">
+      <c r="J5" s="70">
         <v>5</v>
       </c>
-      <c r="K5" s="77">
+      <c r="K5" s="71">
         <v>9</v>
       </c>
     </row>
@@ -5017,13 +5017,13 @@
       <c r="D6" s="54">
         <v>9</v>
       </c>
-      <c r="E6" s="78">
+      <c r="E6" s="72">
         <v>22</v>
       </c>
       <c r="F6" s="19">
         <v>17</v>
       </c>
-      <c r="G6" s="78">
+      <c r="G6" s="72">
         <v>23</v>
       </c>
       <c r="H6" s="19">
@@ -5032,10 +5032,10 @@
       <c r="I6" s="19">
         <v>48</v>
       </c>
-      <c r="J6" s="78">
+      <c r="J6" s="72">
         <v>4</v>
       </c>
-      <c r="K6" s="79">
+      <c r="K6" s="73">
         <v>3</v>
       </c>
     </row>
@@ -5047,7 +5047,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="80">
+      <c r="D7" s="74">
         <v>14</v>
       </c>
       <c r="E7" s="19">
@@ -5056,7 +5056,7 @@
       <c r="F7" s="19">
         <v>3</v>
       </c>
-      <c r="G7" s="78">
+      <c r="G7" s="72">
         <v>3</v>
       </c>
       <c r="H7" s="19">
@@ -5065,10 +5065,10 @@
       <c r="I7" s="19">
         <v>100</v>
       </c>
-      <c r="J7" s="78">
+      <c r="J7" s="72">
         <v>7</v>
       </c>
-      <c r="K7" s="81">
+      <c r="K7" s="75">
         <v>4</v>
       </c>
     </row>
@@ -5078,13 +5078,13 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="76">
         <v>10</v>
       </c>
       <c r="E8" s="44">
         <v>16</v>
       </c>
-      <c r="F8" s="83">
+      <c r="F8" s="77">
         <v>9</v>
       </c>
       <c r="G8" s="44">
@@ -5096,10 +5096,10 @@
       <c r="I8" s="44">
         <v>112</v>
       </c>
-      <c r="J8" s="83">
+      <c r="J8" s="77">
         <v>5</v>
       </c>
-      <c r="K8" s="84">
+      <c r="K8" s="78">
         <v>11</v>
       </c>
     </row>
@@ -5113,16 +5113,16 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="85">
+      <c r="D9" s="79">
         <v>3</v>
       </c>
-      <c r="E9" s="86">
+      <c r="E9" s="80">
         <v>44</v>
       </c>
       <c r="F9" s="35">
         <v>29</v>
       </c>
-      <c r="G9" s="86">
+      <c r="G9" s="80">
         <v>24</v>
       </c>
       <c r="H9" s="35">
@@ -5131,10 +5131,10 @@
       <c r="I9" s="35">
         <v>1</v>
       </c>
-      <c r="J9" s="86">
+      <c r="J9" s="80">
         <v>5</v>
       </c>
-      <c r="K9" s="87">
+      <c r="K9" s="81">
         <v>6</v>
       </c>
     </row>
@@ -5146,16 +5146,16 @@
       <c r="D10" s="54">
         <v>33</v>
       </c>
-      <c r="E10" s="78">
+      <c r="E10" s="72">
         <v>18</v>
       </c>
       <c r="F10" s="19">
         <v>15</v>
       </c>
-      <c r="G10" s="78">
+      <c r="G10" s="72">
         <v>6</v>
       </c>
-      <c r="H10" s="78">
+      <c r="H10" s="72">
         <v>23</v>
       </c>
       <c r="I10" s="19">
@@ -5164,7 +5164,7 @@
       <c r="J10" s="19">
         <v>4</v>
       </c>
-      <c r="K10" s="79">
+      <c r="K10" s="73">
         <v>33</v>
       </c>
     </row>
@@ -5176,7 +5176,7 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="80">
+      <c r="D11" s="74">
         <v>9</v>
       </c>
       <c r="E11" s="19">
@@ -5188,16 +5188,16 @@
       <c r="G11" s="19">
         <v>5</v>
       </c>
-      <c r="H11" s="78">
+      <c r="H11" s="72">
         <v>38</v>
       </c>
-      <c r="I11" s="78">
+      <c r="I11" s="72">
         <v>2</v>
       </c>
       <c r="J11" s="19">
         <v>5</v>
       </c>
-      <c r="K11" s="79">
+      <c r="K11" s="73">
         <v>20</v>
       </c>
     </row>
@@ -5207,10 +5207,10 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="82">
+      <c r="D12" s="76">
         <v>7</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="77">
         <v>16</v>
       </c>
       <c r="F12" s="44">
@@ -5225,10 +5225,10 @@
       <c r="I12" s="44">
         <v>2</v>
       </c>
-      <c r="J12" s="83">
+      <c r="J12" s="77">
         <v>5</v>
       </c>
-      <c r="K12" s="84">
+      <c r="K12" s="78">
         <v>12</v>
       </c>
     </row>
@@ -5242,28 +5242,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="85">
+      <c r="D13" s="79">
         <v>27</v>
       </c>
       <c r="E13" s="35">
         <v>4</v>
       </c>
-      <c r="F13" s="86">
+      <c r="F13" s="80">
         <v>23</v>
       </c>
-      <c r="G13" s="86">
+      <c r="G13" s="80">
         <v>21</v>
       </c>
-      <c r="H13" s="86">
+      <c r="H13" s="80">
         <v>4</v>
       </c>
       <c r="I13" s="35">
         <v>31</v>
       </c>
-      <c r="J13" s="86">
+      <c r="J13" s="80">
         <v>8</v>
       </c>
-      <c r="K13" s="87">
+      <c r="K13" s="81">
         <v>5</v>
       </c>
     </row>
@@ -5272,7 +5272,7 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="80">
+      <c r="D14" s="74">
         <v>35</v>
       </c>
       <c r="E14" s="19">
@@ -5287,13 +5287,13 @@
       <c r="H14" s="19">
         <v>12</v>
       </c>
-      <c r="I14" s="78">
+      <c r="I14" s="72">
         <v>14</v>
       </c>
-      <c r="J14" s="78">
+      <c r="J14" s="72">
         <v>5</v>
       </c>
-      <c r="K14" s="79">
+      <c r="K14" s="73">
         <v>11</v>
       </c>
     </row>
@@ -5305,7 +5305,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="80">
+      <c r="D15" s="74">
         <v>2</v>
       </c>
       <c r="E15" s="19">
@@ -5317,7 +5317,7 @@
       <c r="G15" s="19">
         <v>2</v>
       </c>
-      <c r="H15" s="78">
+      <c r="H15" s="72">
         <v>2</v>
       </c>
       <c r="I15" s="19">
@@ -5326,7 +5326,7 @@
       <c r="J15" s="19">
         <v>2</v>
       </c>
-      <c r="K15" s="81">
+      <c r="K15" s="75">
         <v>2</v>
       </c>
     </row>
@@ -5336,10 +5336,10 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="82">
-        <v>2</v>
-      </c>
-      <c r="E16" s="83">
+      <c r="D16" s="76">
+        <v>2</v>
+      </c>
+      <c r="E16" s="77">
         <v>2</v>
       </c>
       <c r="F16" s="44">
@@ -5348,16 +5348,16 @@
       <c r="G16" s="44">
         <v>2</v>
       </c>
-      <c r="H16" s="83">
-        <v>2</v>
-      </c>
-      <c r="I16" s="83">
+      <c r="H16" s="77">
+        <v>2</v>
+      </c>
+      <c r="I16" s="77">
         <v>2</v>
       </c>
       <c r="J16" s="44">
         <v>2</v>
       </c>
-      <c r="K16" s="88">
+      <c r="K16" s="82">
         <v>2</v>
       </c>
     </row>
@@ -5371,13 +5371,13 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="85">
+      <c r="D17" s="79">
         <v>112</v>
       </c>
-      <c r="E17" s="86">
+      <c r="E17" s="80">
         <v>82</v>
       </c>
-      <c r="F17" s="86">
+      <c r="F17" s="80">
         <v>6</v>
       </c>
       <c r="G17" s="35">
@@ -5386,13 +5386,13 @@
       <c r="H17" s="35">
         <v>77</v>
       </c>
-      <c r="I17" s="86">
+      <c r="I17" s="80">
         <v>3</v>
       </c>
       <c r="J17" s="35">
         <v>24</v>
       </c>
-      <c r="K17" s="87">
+      <c r="K17" s="81">
         <v>78</v>
       </c>
     </row>
@@ -5401,19 +5401,19 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="80">
+      <c r="D18" s="74">
         <v>108</v>
       </c>
       <c r="E18" s="19">
         <v>36</v>
       </c>
-      <c r="F18" s="78">
+      <c r="F18" s="72">
         <v>23</v>
       </c>
       <c r="G18" s="19">
         <v>38</v>
       </c>
-      <c r="H18" s="78">
+      <c r="H18" s="72">
         <v>50</v>
       </c>
       <c r="I18" s="19">
@@ -5422,7 +5422,7 @@
       <c r="J18" s="19">
         <v>7</v>
       </c>
-      <c r="K18" s="79">
+      <c r="K18" s="73">
         <v>17</v>
       </c>
     </row>
@@ -5440,7 +5440,7 @@
       <c r="E19" s="19">
         <v>3</v>
       </c>
-      <c r="F19" s="78">
+      <c r="F19" s="72">
         <v>12</v>
       </c>
       <c r="G19" s="19">
@@ -5452,10 +5452,10 @@
       <c r="I19" s="19">
         <v>10</v>
       </c>
-      <c r="J19" s="78">
+      <c r="J19" s="72">
         <v>12</v>
       </c>
-      <c r="K19" s="81">
+      <c r="K19" s="75">
         <v>18</v>
       </c>
     </row>
@@ -5465,10 +5465,10 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="82">
+      <c r="D20" s="76">
         <v>8</v>
       </c>
-      <c r="E20" s="83">
+      <c r="E20" s="77">
         <v>9</v>
       </c>
       <c r="F20" s="44">
@@ -5477,16 +5477,16 @@
       <c r="G20" s="44">
         <v>9</v>
       </c>
-      <c r="H20" s="83">
+      <c r="H20" s="77">
         <v>9</v>
       </c>
       <c r="I20" s="44">
         <v>12</v>
       </c>
-      <c r="J20" s="83">
+      <c r="J20" s="77">
         <v>11</v>
       </c>
-      <c r="K20" s="88">
+      <c r="K20" s="82">
         <v>4</v>
       </c>
     </row>
@@ -5676,7 +5676,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5694,19 +5694,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5754,28 +5754,28 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="74">
+      <c r="D5" s="68">
         <v>6.1</v>
       </c>
-      <c r="E5" s="75">
+      <c r="E5" s="69">
         <v>9.1</v>
       </c>
-      <c r="F5" s="76">
+      <c r="F5" s="70">
         <v>14.6</v>
       </c>
-      <c r="G5" s="76">
+      <c r="G5" s="70">
         <v>14.2</v>
       </c>
-      <c r="H5" s="75">
+      <c r="H5" s="69">
         <v>15.5</v>
       </c>
-      <c r="I5" s="75">
+      <c r="I5" s="69">
         <v>60</v>
       </c>
-      <c r="J5" s="76">
+      <c r="J5" s="70">
         <v>7</v>
       </c>
-      <c r="K5" s="77">
+      <c r="K5" s="71">
         <v>10.7</v>
       </c>
     </row>
@@ -5787,13 +5787,13 @@
       <c r="D6" s="54">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E6" s="78">
+      <c r="E6" s="72">
         <v>27.6</v>
       </c>
       <c r="F6" s="19">
         <v>9</v>
       </c>
-      <c r="G6" s="78">
+      <c r="G6" s="72">
         <v>18.8</v>
       </c>
       <c r="H6" s="19">
@@ -5802,10 +5802,10 @@
       <c r="I6" s="19">
         <v>74.400000000000006</v>
       </c>
-      <c r="J6" s="78">
+      <c r="J6" s="72">
         <v>7</v>
       </c>
-      <c r="K6" s="79">
+      <c r="K6" s="73">
         <v>19</v>
       </c>
     </row>
@@ -5817,7 +5817,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="80">
+      <c r="D7" s="74">
         <v>8.5</v>
       </c>
       <c r="E7" s="19">
@@ -5826,7 +5826,7 @@
       <c r="F7" s="19">
         <v>9.6999999999999993</v>
       </c>
-      <c r="G7" s="78">
+      <c r="G7" s="72">
         <v>6.9</v>
       </c>
       <c r="H7" s="19">
@@ -5835,10 +5835,10 @@
       <c r="I7" s="19">
         <v>29.8</v>
       </c>
-      <c r="J7" s="78">
+      <c r="J7" s="72">
         <v>6.5</v>
       </c>
-      <c r="K7" s="81">
+      <c r="K7" s="75">
         <v>13.3</v>
       </c>
     </row>
@@ -5848,13 +5848,13 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="76">
         <v>10.199999999999999</v>
       </c>
       <c r="E8" s="44">
         <v>19.5</v>
       </c>
-      <c r="F8" s="83">
+      <c r="F8" s="77">
         <v>10.8</v>
       </c>
       <c r="G8" s="44">
@@ -5866,10 +5866,10 @@
       <c r="I8" s="44">
         <v>72.7</v>
       </c>
-      <c r="J8" s="83">
+      <c r="J8" s="77">
         <v>6.5</v>
       </c>
-      <c r="K8" s="84">
+      <c r="K8" s="78">
         <v>12.6</v>
       </c>
     </row>
@@ -5883,16 +5883,16 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="85">
+      <c r="D9" s="79">
         <v>11.9</v>
       </c>
-      <c r="E9" s="86">
+      <c r="E9" s="80">
         <v>13</v>
       </c>
       <c r="F9" s="35">
         <v>12.8</v>
       </c>
-      <c r="G9" s="86">
+      <c r="G9" s="80">
         <v>19.2</v>
       </c>
       <c r="H9" s="35">
@@ -5901,10 +5901,10 @@
       <c r="I9" s="35">
         <v>1</v>
       </c>
-      <c r="J9" s="86">
+      <c r="J9" s="80">
         <v>16</v>
       </c>
-      <c r="K9" s="87">
+      <c r="K9" s="81">
         <v>10.6</v>
       </c>
     </row>
@@ -5916,16 +5916,16 @@
       <c r="D10" s="54">
         <v>15.1</v>
       </c>
-      <c r="E10" s="78">
+      <c r="E10" s="72">
         <v>16.2</v>
       </c>
       <c r="F10" s="19">
         <v>15.2</v>
       </c>
-      <c r="G10" s="78">
+      <c r="G10" s="72">
         <v>13</v>
       </c>
-      <c r="H10" s="78">
+      <c r="H10" s="72">
         <v>27.2</v>
       </c>
       <c r="I10" s="19">
@@ -5934,7 +5934,7 @@
       <c r="J10" s="19">
         <v>6.3</v>
       </c>
-      <c r="K10" s="79">
+      <c r="K10" s="73">
         <v>18.899999999999999</v>
       </c>
     </row>
@@ -5946,7 +5946,7 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="80">
+      <c r="D11" s="74">
         <v>12.5</v>
       </c>
       <c r="E11" s="19">
@@ -5958,16 +5958,16 @@
       <c r="G11" s="19">
         <v>11.3</v>
       </c>
-      <c r="H11" s="78">
+      <c r="H11" s="72">
         <v>18.5</v>
       </c>
-      <c r="I11" s="78">
+      <c r="I11" s="72">
         <v>2</v>
       </c>
       <c r="J11" s="19">
         <v>4.9000000000000004</v>
       </c>
-      <c r="K11" s="79">
+      <c r="K11" s="73">
         <v>8.5</v>
       </c>
     </row>
@@ -5977,10 +5977,10 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="82">
+      <c r="D12" s="76">
         <v>9.1</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="77">
         <v>19.3</v>
       </c>
       <c r="F12" s="44">
@@ -5995,10 +5995,10 @@
       <c r="I12" s="44">
         <v>2</v>
       </c>
-      <c r="J12" s="83">
+      <c r="J12" s="77">
         <v>9</v>
       </c>
-      <c r="K12" s="84">
+      <c r="K12" s="78">
         <v>17.899999999999999</v>
       </c>
     </row>
@@ -6012,28 +6012,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="85">
+      <c r="D13" s="79">
         <v>12.7</v>
       </c>
       <c r="E13" s="35">
         <v>15.4</v>
       </c>
-      <c r="F13" s="86">
+      <c r="F13" s="80">
         <v>17.7</v>
       </c>
-      <c r="G13" s="86">
+      <c r="G13" s="80">
         <v>11.6</v>
       </c>
-      <c r="H13" s="86">
+      <c r="H13" s="80">
         <v>11.6</v>
       </c>
       <c r="I13" s="35">
         <v>15.4</v>
       </c>
-      <c r="J13" s="86">
+      <c r="J13" s="80">
         <v>13.9</v>
       </c>
-      <c r="K13" s="87">
+      <c r="K13" s="81">
         <v>8.6999999999999993</v>
       </c>
     </row>
@@ -6042,7 +6042,7 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="80">
+      <c r="D14" s="74">
         <v>13.7</v>
       </c>
       <c r="E14" s="19">
@@ -6057,13 +6057,13 @@
       <c r="H14" s="19">
         <v>15.2</v>
       </c>
-      <c r="I14" s="78">
+      <c r="I14" s="72">
         <v>19</v>
       </c>
-      <c r="J14" s="78">
+      <c r="J14" s="72">
         <v>7.5</v>
       </c>
-      <c r="K14" s="79">
+      <c r="K14" s="73">
         <v>15.6</v>
       </c>
     </row>
@@ -6075,7 +6075,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="80">
+      <c r="D15" s="74">
         <v>2</v>
       </c>
       <c r="E15" s="19">
@@ -6087,7 +6087,7 @@
       <c r="G15" s="19">
         <v>2</v>
       </c>
-      <c r="H15" s="78">
+      <c r="H15" s="72">
         <v>2</v>
       </c>
       <c r="I15" s="19">
@@ -6096,7 +6096,7 @@
       <c r="J15" s="19">
         <v>2</v>
       </c>
-      <c r="K15" s="81">
+      <c r="K15" s="75">
         <v>2</v>
       </c>
     </row>
@@ -6106,10 +6106,10 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="82">
-        <v>2</v>
-      </c>
-      <c r="E16" s="83">
+      <c r="D16" s="76">
+        <v>2</v>
+      </c>
+      <c r="E16" s="77">
         <v>2</v>
       </c>
       <c r="F16" s="44">
@@ -6118,16 +6118,16 @@
       <c r="G16" s="44">
         <v>2</v>
       </c>
-      <c r="H16" s="83">
-        <v>2</v>
-      </c>
-      <c r="I16" s="83">
+      <c r="H16" s="77">
+        <v>2</v>
+      </c>
+      <c r="I16" s="77">
         <v>2</v>
       </c>
       <c r="J16" s="44">
         <v>2</v>
       </c>
-      <c r="K16" s="88">
+      <c r="K16" s="82">
         <v>2</v>
       </c>
     </row>
@@ -6141,13 +6141,13 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="85">
+      <c r="D17" s="79">
         <v>75.5</v>
       </c>
-      <c r="E17" s="86">
+      <c r="E17" s="80">
         <v>98.2</v>
       </c>
-      <c r="F17" s="86">
+      <c r="F17" s="80">
         <v>15.1</v>
       </c>
       <c r="G17" s="35">
@@ -6156,13 +6156,13 @@
       <c r="H17" s="35">
         <v>46.2</v>
       </c>
-      <c r="I17" s="86">
+      <c r="I17" s="80">
         <v>10.4</v>
       </c>
       <c r="J17" s="35">
         <v>7.7</v>
       </c>
-      <c r="K17" s="87">
+      <c r="K17" s="81">
         <v>75</v>
       </c>
     </row>
@@ -6171,19 +6171,19 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="80">
+      <c r="D18" s="74">
         <v>91</v>
       </c>
       <c r="E18" s="19">
         <v>68.599999999999994</v>
       </c>
-      <c r="F18" s="78">
+      <c r="F18" s="72">
         <v>14.7</v>
       </c>
       <c r="G18" s="19">
         <v>42.2</v>
       </c>
-      <c r="H18" s="78">
+      <c r="H18" s="72">
         <v>53.5</v>
       </c>
       <c r="I18" s="19">
@@ -6192,7 +6192,7 @@
       <c r="J18" s="19">
         <v>5.7</v>
       </c>
-      <c r="K18" s="79">
+      <c r="K18" s="73">
         <v>66.5</v>
       </c>
     </row>
@@ -6210,7 +6210,7 @@
       <c r="E19" s="19">
         <v>13.4</v>
       </c>
-      <c r="F19" s="78">
+      <c r="F19" s="72">
         <v>9.5</v>
       </c>
       <c r="G19" s="19">
@@ -6222,10 +6222,10 @@
       <c r="I19" s="19">
         <v>10.8</v>
       </c>
-      <c r="J19" s="78">
+      <c r="J19" s="72">
         <v>9.9</v>
       </c>
-      <c r="K19" s="81">
+      <c r="K19" s="75">
         <v>6.5</v>
       </c>
     </row>
@@ -6235,10 +6235,10 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="82">
+      <c r="D20" s="76">
         <v>10.7</v>
       </c>
-      <c r="E20" s="83">
+      <c r="E20" s="77">
         <v>15.2</v>
       </c>
       <c r="F20" s="44">
@@ -6247,16 +6247,16 @@
       <c r="G20" s="44">
         <v>17.399999999999999</v>
       </c>
-      <c r="H20" s="83">
+      <c r="H20" s="77">
         <v>10.199999999999999</v>
       </c>
       <c r="I20" s="44">
         <v>10</v>
       </c>
-      <c r="J20" s="83">
+      <c r="J20" s="77">
         <v>9.1</v>
       </c>
-      <c r="K20" s="88">
+      <c r="K20" s="82">
         <v>15.3</v>
       </c>
     </row>
@@ -6446,7 +6446,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6464,19 +6464,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6524,28 +6524,28 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="74">
-        <v>1</v>
-      </c>
-      <c r="E5" s="75">
-        <v>1</v>
-      </c>
-      <c r="F5" s="76">
-        <v>1</v>
-      </c>
-      <c r="G5" s="76">
-        <v>1</v>
-      </c>
-      <c r="H5" s="75">
-        <v>1</v>
-      </c>
-      <c r="I5" s="75">
-        <v>1</v>
-      </c>
-      <c r="J5" s="76">
-        <v>1</v>
-      </c>
-      <c r="K5" s="77">
+      <c r="D5" s="68">
+        <v>1</v>
+      </c>
+      <c r="E5" s="69">
+        <v>1</v>
+      </c>
+      <c r="F5" s="70">
+        <v>1</v>
+      </c>
+      <c r="G5" s="70">
+        <v>1</v>
+      </c>
+      <c r="H5" s="69">
+        <v>1</v>
+      </c>
+      <c r="I5" s="69">
+        <v>1</v>
+      </c>
+      <c r="J5" s="70">
+        <v>1</v>
+      </c>
+      <c r="K5" s="71">
         <v>1</v>
       </c>
     </row>
@@ -6557,13 +6557,13 @@
       <c r="D6" s="54">
         <v>2</v>
       </c>
-      <c r="E6" s="78">
+      <c r="E6" s="72">
         <v>6</v>
       </c>
       <c r="F6" s="19">
         <v>9</v>
       </c>
-      <c r="G6" s="78">
+      <c r="G6" s="72">
         <v>7</v>
       </c>
       <c r="H6" s="19">
@@ -6572,10 +6572,10 @@
       <c r="I6" s="19">
         <v>4</v>
       </c>
-      <c r="J6" s="78">
-        <v>2</v>
-      </c>
-      <c r="K6" s="79">
+      <c r="J6" s="72">
+        <v>2</v>
+      </c>
+      <c r="K6" s="73">
         <v>2</v>
       </c>
     </row>
@@ -6587,7 +6587,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="80">
+      <c r="D7" s="74">
         <v>1</v>
       </c>
       <c r="E7" s="19">
@@ -6596,7 +6596,7 @@
       <c r="F7" s="19">
         <v>1</v>
       </c>
-      <c r="G7" s="78">
+      <c r="G7" s="72">
         <v>1</v>
       </c>
       <c r="H7" s="19">
@@ -6605,10 +6605,10 @@
       <c r="I7" s="19">
         <v>1</v>
       </c>
-      <c r="J7" s="78">
-        <v>1</v>
-      </c>
-      <c r="K7" s="81">
+      <c r="J7" s="72">
+        <v>1</v>
+      </c>
+      <c r="K7" s="75">
         <v>1</v>
       </c>
     </row>
@@ -6618,13 +6618,13 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="76">
         <v>3</v>
       </c>
       <c r="E8" s="44">
         <v>9</v>
       </c>
-      <c r="F8" s="83">
+      <c r="F8" s="77">
         <v>6</v>
       </c>
       <c r="G8" s="44">
@@ -6636,10 +6636,10 @@
       <c r="I8" s="44">
         <v>4</v>
       </c>
-      <c r="J8" s="83">
+      <c r="J8" s="77">
         <v>4</v>
       </c>
-      <c r="K8" s="84">
+      <c r="K8" s="78">
         <v>9</v>
       </c>
     </row>
@@ -6653,16 +6653,16 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="85">
-        <v>1</v>
-      </c>
-      <c r="E9" s="86">
+      <c r="D9" s="79">
+        <v>1</v>
+      </c>
+      <c r="E9" s="80">
         <v>1</v>
       </c>
       <c r="F9" s="35">
         <v>1</v>
       </c>
-      <c r="G9" s="86">
+      <c r="G9" s="80">
         <v>1</v>
       </c>
       <c r="H9" s="35">
@@ -6671,10 +6671,10 @@
       <c r="I9" s="35">
         <v>1</v>
       </c>
-      <c r="J9" s="86">
-        <v>1</v>
-      </c>
-      <c r="K9" s="87">
+      <c r="J9" s="80">
+        <v>1</v>
+      </c>
+      <c r="K9" s="81">
         <v>1</v>
       </c>
     </row>
@@ -6686,16 +6686,16 @@
       <c r="D10" s="54">
         <v>8</v>
       </c>
-      <c r="E10" s="78">
+      <c r="E10" s="72">
         <v>10</v>
       </c>
       <c r="F10" s="19">
         <v>7</v>
       </c>
-      <c r="G10" s="78">
+      <c r="G10" s="72">
         <v>3</v>
       </c>
-      <c r="H10" s="78">
+      <c r="H10" s="72">
         <v>3</v>
       </c>
       <c r="I10" s="19">
@@ -6704,7 +6704,7 @@
       <c r="J10" s="19">
         <v>9</v>
       </c>
-      <c r="K10" s="79">
+      <c r="K10" s="73">
         <v>10</v>
       </c>
     </row>
@@ -6716,7 +6716,7 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="80">
+      <c r="D11" s="74">
         <v>1</v>
       </c>
       <c r="E11" s="19">
@@ -6728,16 +6728,16 @@
       <c r="G11" s="19">
         <v>1</v>
       </c>
-      <c r="H11" s="78">
-        <v>1</v>
-      </c>
-      <c r="I11" s="78">
+      <c r="H11" s="72">
+        <v>1</v>
+      </c>
+      <c r="I11" s="72">
         <v>1</v>
       </c>
       <c r="J11" s="19">
         <v>1</v>
       </c>
-      <c r="K11" s="79">
+      <c r="K11" s="73">
         <v>1</v>
       </c>
     </row>
@@ -6747,10 +6747,10 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="82">
+      <c r="D12" s="76">
         <v>9</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="77">
         <v>4</v>
       </c>
       <c r="F12" s="44">
@@ -6765,10 +6765,10 @@
       <c r="I12" s="44">
         <v>2</v>
       </c>
-      <c r="J12" s="83">
+      <c r="J12" s="77">
         <v>9</v>
       </c>
-      <c r="K12" s="84">
+      <c r="K12" s="78">
         <v>4</v>
       </c>
     </row>
@@ -6782,28 +6782,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="85">
+      <c r="D13" s="79">
         <v>1</v>
       </c>
       <c r="E13" s="35">
         <v>1</v>
       </c>
-      <c r="F13" s="86">
-        <v>1</v>
-      </c>
-      <c r="G13" s="86">
-        <v>1</v>
-      </c>
-      <c r="H13" s="86">
+      <c r="F13" s="80">
+        <v>1</v>
+      </c>
+      <c r="G13" s="80">
+        <v>1</v>
+      </c>
+      <c r="H13" s="80">
         <v>1</v>
       </c>
       <c r="I13" s="35">
         <v>1</v>
       </c>
-      <c r="J13" s="86">
-        <v>1</v>
-      </c>
-      <c r="K13" s="87">
+      <c r="J13" s="80">
+        <v>1</v>
+      </c>
+      <c r="K13" s="81">
         <v>1</v>
       </c>
     </row>
@@ -6812,7 +6812,7 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="80">
+      <c r="D14" s="74">
         <v>9</v>
       </c>
       <c r="E14" s="19">
@@ -6827,13 +6827,13 @@
       <c r="H14" s="19">
         <v>5</v>
       </c>
-      <c r="I14" s="78">
+      <c r="I14" s="72">
         <v>9</v>
       </c>
-      <c r="J14" s="78">
+      <c r="J14" s="72">
         <v>9</v>
       </c>
-      <c r="K14" s="79">
+      <c r="K14" s="73">
         <v>4</v>
       </c>
     </row>
@@ -6845,7 +6845,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="80">
+      <c r="D15" s="74">
         <v>1</v>
       </c>
       <c r="E15" s="19">
@@ -6857,7 +6857,7 @@
       <c r="G15" s="19">
         <v>1</v>
       </c>
-      <c r="H15" s="78">
+      <c r="H15" s="72">
         <v>1</v>
       </c>
       <c r="I15" s="19">
@@ -6866,7 +6866,7 @@
       <c r="J15" s="19">
         <v>1</v>
       </c>
-      <c r="K15" s="81">
+      <c r="K15" s="75">
         <v>1</v>
       </c>
     </row>
@@ -6876,10 +6876,10 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="82">
+      <c r="D16" s="76">
         <v>3</v>
       </c>
-      <c r="E16" s="83">
+      <c r="E16" s="77">
         <v>2</v>
       </c>
       <c r="F16" s="44">
@@ -6888,16 +6888,16 @@
       <c r="G16" s="44">
         <v>8</v>
       </c>
-      <c r="H16" s="83">
+      <c r="H16" s="77">
         <v>7</v>
       </c>
-      <c r="I16" s="83">
+      <c r="I16" s="77">
         <v>5</v>
       </c>
       <c r="J16" s="44">
         <v>4</v>
       </c>
-      <c r="K16" s="88">
+      <c r="K16" s="82">
         <v>10</v>
       </c>
     </row>
@@ -6911,13 +6911,13 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="85">
-        <v>1</v>
-      </c>
-      <c r="E17" s="86">
-        <v>1</v>
-      </c>
-      <c r="F17" s="86">
+      <c r="D17" s="79">
+        <v>1</v>
+      </c>
+      <c r="E17" s="80">
+        <v>1</v>
+      </c>
+      <c r="F17" s="80">
         <v>1</v>
       </c>
       <c r="G17" s="35">
@@ -6926,13 +6926,13 @@
       <c r="H17" s="35">
         <v>1</v>
       </c>
-      <c r="I17" s="86">
+      <c r="I17" s="80">
         <v>1</v>
       </c>
       <c r="J17" s="35">
         <v>1</v>
       </c>
-      <c r="K17" s="87">
+      <c r="K17" s="81">
         <v>1</v>
       </c>
     </row>
@@ -6941,19 +6941,19 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="80">
+      <c r="D18" s="74">
         <v>6</v>
       </c>
       <c r="E18" s="19">
         <v>9</v>
       </c>
-      <c r="F18" s="78">
+      <c r="F18" s="72">
         <v>5</v>
       </c>
       <c r="G18" s="19">
         <v>9</v>
       </c>
-      <c r="H18" s="78">
+      <c r="H18" s="72">
         <v>7</v>
       </c>
       <c r="I18" s="19">
@@ -6962,7 +6962,7 @@
       <c r="J18" s="19">
         <v>5</v>
       </c>
-      <c r="K18" s="79">
+      <c r="K18" s="73">
         <v>2</v>
       </c>
     </row>
@@ -6980,7 +6980,7 @@
       <c r="E19" s="19">
         <v>1</v>
       </c>
-      <c r="F19" s="78">
+      <c r="F19" s="72">
         <v>1</v>
       </c>
       <c r="G19" s="19">
@@ -6992,10 +6992,10 @@
       <c r="I19" s="19">
         <v>1</v>
       </c>
-      <c r="J19" s="78">
-        <v>1</v>
-      </c>
-      <c r="K19" s="81">
+      <c r="J19" s="72">
+        <v>1</v>
+      </c>
+      <c r="K19" s="75">
         <v>1</v>
       </c>
     </row>
@@ -7005,10 +7005,10 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="82">
+      <c r="D20" s="76">
         <v>10</v>
       </c>
-      <c r="E20" s="83">
+      <c r="E20" s="77">
         <v>5</v>
       </c>
       <c r="F20" s="44">
@@ -7017,16 +7017,16 @@
       <c r="G20" s="44">
         <v>6</v>
       </c>
-      <c r="H20" s="83">
+      <c r="H20" s="77">
         <v>5</v>
       </c>
       <c r="I20" s="44">
         <v>2</v>
       </c>
-      <c r="J20" s="83">
+      <c r="J20" s="77">
         <v>8</v>
       </c>
-      <c r="K20" s="88">
+      <c r="K20" s="82">
         <v>8</v>
       </c>
     </row>
@@ -7216,7 +7216,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7234,19 +7234,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7294,28 +7294,28 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="74">
-        <v>1</v>
-      </c>
-      <c r="E5" s="75">
-        <v>1</v>
-      </c>
-      <c r="F5" s="76">
-        <v>1</v>
-      </c>
-      <c r="G5" s="76">
-        <v>1</v>
-      </c>
-      <c r="H5" s="75">
-        <v>1</v>
-      </c>
-      <c r="I5" s="75">
-        <v>1</v>
-      </c>
-      <c r="J5" s="76">
-        <v>1</v>
-      </c>
-      <c r="K5" s="77">
+      <c r="D5" s="68">
+        <v>1</v>
+      </c>
+      <c r="E5" s="69">
+        <v>1</v>
+      </c>
+      <c r="F5" s="70">
+        <v>1</v>
+      </c>
+      <c r="G5" s="70">
+        <v>1</v>
+      </c>
+      <c r="H5" s="69">
+        <v>1</v>
+      </c>
+      <c r="I5" s="69">
+        <v>1</v>
+      </c>
+      <c r="J5" s="70">
+        <v>1</v>
+      </c>
+      <c r="K5" s="71">
         <v>1</v>
       </c>
     </row>
@@ -7327,13 +7327,13 @@
       <c r="D6" s="54">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E6" s="78">
+      <c r="E6" s="72">
         <v>5.4</v>
       </c>
       <c r="F6" s="19">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G6" s="78">
+      <c r="G6" s="72">
         <v>5.5</v>
       </c>
       <c r="H6" s="19">
@@ -7342,10 +7342,10 @@
       <c r="I6" s="19">
         <v>4</v>
       </c>
-      <c r="J6" s="78">
+      <c r="J6" s="72">
         <v>4.3</v>
       </c>
-      <c r="K6" s="79">
+      <c r="K6" s="73">
         <v>4.8</v>
       </c>
     </row>
@@ -7357,7 +7357,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="80">
+      <c r="D7" s="74">
         <v>1</v>
       </c>
       <c r="E7" s="19">
@@ -7366,7 +7366,7 @@
       <c r="F7" s="19">
         <v>1</v>
       </c>
-      <c r="G7" s="78">
+      <c r="G7" s="72">
         <v>1</v>
       </c>
       <c r="H7" s="19">
@@ -7375,10 +7375,10 @@
       <c r="I7" s="19">
         <v>1</v>
       </c>
-      <c r="J7" s="78">
-        <v>1</v>
-      </c>
-      <c r="K7" s="81">
+      <c r="J7" s="72">
+        <v>1</v>
+      </c>
+      <c r="K7" s="75">
         <v>1</v>
       </c>
     </row>
@@ -7388,13 +7388,13 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="76">
         <v>4.5</v>
       </c>
       <c r="E8" s="44">
         <v>7.5</v>
       </c>
-      <c r="F8" s="83">
+      <c r="F8" s="77">
         <v>4.5999999999999996</v>
       </c>
       <c r="G8" s="44">
@@ -7406,10 +7406,10 @@
       <c r="I8" s="44">
         <v>6</v>
       </c>
-      <c r="J8" s="83">
+      <c r="J8" s="77">
         <v>6.3</v>
       </c>
-      <c r="K8" s="84">
+      <c r="K8" s="78">
         <v>5.6</v>
       </c>
     </row>
@@ -7423,16 +7423,16 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="85">
-        <v>1</v>
-      </c>
-      <c r="E9" s="86">
+      <c r="D9" s="79">
+        <v>1</v>
+      </c>
+      <c r="E9" s="80">
         <v>1</v>
       </c>
       <c r="F9" s="35">
         <v>1</v>
       </c>
-      <c r="G9" s="86">
+      <c r="G9" s="80">
         <v>1</v>
       </c>
       <c r="H9" s="35">
@@ -7441,10 +7441,10 @@
       <c r="I9" s="35">
         <v>1</v>
       </c>
-      <c r="J9" s="86">
-        <v>1</v>
-      </c>
-      <c r="K9" s="87">
+      <c r="J9" s="80">
+        <v>1</v>
+      </c>
+      <c r="K9" s="81">
         <v>1</v>
       </c>
     </row>
@@ -7456,16 +7456,16 @@
       <c r="D10" s="54">
         <v>6.1</v>
       </c>
-      <c r="E10" s="78">
+      <c r="E10" s="72">
         <v>7.4</v>
       </c>
       <c r="F10" s="19">
         <v>7</v>
       </c>
-      <c r="G10" s="78">
+      <c r="G10" s="72">
         <v>5.9</v>
       </c>
-      <c r="H10" s="78">
+      <c r="H10" s="72">
         <v>5.9</v>
       </c>
       <c r="I10" s="19">
@@ -7474,7 +7474,7 @@
       <c r="J10" s="19">
         <v>5.0999999999999996</v>
       </c>
-      <c r="K10" s="79">
+      <c r="K10" s="73">
         <v>6</v>
       </c>
     </row>
@@ -7486,7 +7486,7 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="80">
+      <c r="D11" s="74">
         <v>1</v>
       </c>
       <c r="E11" s="19">
@@ -7498,16 +7498,16 @@
       <c r="G11" s="19">
         <v>1</v>
       </c>
-      <c r="H11" s="78">
-        <v>1</v>
-      </c>
-      <c r="I11" s="78">
+      <c r="H11" s="72">
+        <v>1</v>
+      </c>
+      <c r="I11" s="72">
         <v>1</v>
       </c>
       <c r="J11" s="19">
         <v>1</v>
       </c>
-      <c r="K11" s="79">
+      <c r="K11" s="73">
         <v>1</v>
       </c>
     </row>
@@ -7517,10 +7517,10 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="82">
+      <c r="D12" s="76">
         <v>5.9</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="77">
         <v>5.3</v>
       </c>
       <c r="F12" s="44">
@@ -7535,10 +7535,10 @@
       <c r="I12" s="44">
         <v>5.4</v>
       </c>
-      <c r="J12" s="83">
+      <c r="J12" s="77">
         <v>5.7</v>
       </c>
-      <c r="K12" s="84">
+      <c r="K12" s="78">
         <v>5.3</v>
       </c>
     </row>
@@ -7552,28 +7552,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="85">
+      <c r="D13" s="79">
         <v>1</v>
       </c>
       <c r="E13" s="35">
         <v>1</v>
       </c>
-      <c r="F13" s="86">
-        <v>1</v>
-      </c>
-      <c r="G13" s="86">
-        <v>1</v>
-      </c>
-      <c r="H13" s="86">
+      <c r="F13" s="80">
+        <v>1</v>
+      </c>
+      <c r="G13" s="80">
+        <v>1</v>
+      </c>
+      <c r="H13" s="80">
         <v>1</v>
       </c>
       <c r="I13" s="35">
         <v>1</v>
       </c>
-      <c r="J13" s="86">
-        <v>1</v>
-      </c>
-      <c r="K13" s="87">
+      <c r="J13" s="80">
+        <v>1</v>
+      </c>
+      <c r="K13" s="81">
         <v>1</v>
       </c>
     </row>
@@ -7582,7 +7582,7 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="80">
+      <c r="D14" s="74">
         <v>5</v>
       </c>
       <c r="E14" s="19">
@@ -7597,13 +7597,13 @@
       <c r="H14" s="19">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I14" s="78">
+      <c r="I14" s="72">
         <v>6.4</v>
       </c>
-      <c r="J14" s="78">
+      <c r="J14" s="72">
         <v>6.7</v>
       </c>
-      <c r="K14" s="79">
+      <c r="K14" s="73">
         <v>6.3</v>
       </c>
     </row>
@@ -7615,7 +7615,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="80">
+      <c r="D15" s="74">
         <v>1</v>
       </c>
       <c r="E15" s="19">
@@ -7627,7 +7627,7 @@
       <c r="G15" s="19">
         <v>1</v>
       </c>
-      <c r="H15" s="78">
+      <c r="H15" s="72">
         <v>1</v>
       </c>
       <c r="I15" s="19">
@@ -7636,7 +7636,7 @@
       <c r="J15" s="19">
         <v>1</v>
       </c>
-      <c r="K15" s="81">
+      <c r="K15" s="75">
         <v>1</v>
       </c>
     </row>
@@ -7646,10 +7646,10 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="82">
+      <c r="D16" s="76">
         <v>6.2</v>
       </c>
-      <c r="E16" s="83">
+      <c r="E16" s="77">
         <v>5.2</v>
       </c>
       <c r="F16" s="44">
@@ -7658,16 +7658,16 @@
       <c r="G16" s="44">
         <v>7.5</v>
       </c>
-      <c r="H16" s="83">
+      <c r="H16" s="77">
         <v>7.3</v>
       </c>
-      <c r="I16" s="83">
+      <c r="I16" s="77">
         <v>6.1</v>
       </c>
       <c r="J16" s="44">
         <v>6.6</v>
       </c>
-      <c r="K16" s="88">
+      <c r="K16" s="82">
         <v>5.7</v>
       </c>
     </row>
@@ -7681,13 +7681,13 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="85">
-        <v>1</v>
-      </c>
-      <c r="E17" s="86">
-        <v>1</v>
-      </c>
-      <c r="F17" s="86">
+      <c r="D17" s="79">
+        <v>1</v>
+      </c>
+      <c r="E17" s="80">
+        <v>1</v>
+      </c>
+      <c r="F17" s="80">
         <v>1</v>
       </c>
       <c r="G17" s="35">
@@ -7696,13 +7696,13 @@
       <c r="H17" s="35">
         <v>1</v>
       </c>
-      <c r="I17" s="86">
+      <c r="I17" s="80">
         <v>1</v>
       </c>
       <c r="J17" s="35">
         <v>1</v>
       </c>
-      <c r="K17" s="87">
+      <c r="K17" s="81">
         <v>1</v>
       </c>
     </row>
@@ -7711,19 +7711,19 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="80">
+      <c r="D18" s="74">
         <v>6.1</v>
       </c>
       <c r="E18" s="19">
         <v>6</v>
       </c>
-      <c r="F18" s="78">
+      <c r="F18" s="72">
         <v>5.8</v>
       </c>
       <c r="G18" s="19">
         <v>6.4</v>
       </c>
-      <c r="H18" s="78">
+      <c r="H18" s="72">
         <v>5.9</v>
       </c>
       <c r="I18" s="19">
@@ -7732,7 +7732,7 @@
       <c r="J18" s="19">
         <v>5.6</v>
       </c>
-      <c r="K18" s="79">
+      <c r="K18" s="73">
         <v>5.4</v>
       </c>
     </row>
@@ -7750,7 +7750,7 @@
       <c r="E19" s="19">
         <v>1</v>
       </c>
-      <c r="F19" s="78">
+      <c r="F19" s="72">
         <v>1</v>
       </c>
       <c r="G19" s="19">
@@ -7762,10 +7762,10 @@
       <c r="I19" s="19">
         <v>1</v>
       </c>
-      <c r="J19" s="78">
-        <v>1</v>
-      </c>
-      <c r="K19" s="81">
+      <c r="J19" s="72">
+        <v>1</v>
+      </c>
+      <c r="K19" s="75">
         <v>1</v>
       </c>
     </row>
@@ -7775,10 +7775,10 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="82">
+      <c r="D20" s="76">
         <v>6.4</v>
       </c>
-      <c r="E20" s="83">
+      <c r="E20" s="77">
         <v>6.1</v>
       </c>
       <c r="F20" s="44">
@@ -7787,16 +7787,16 @@
       <c r="G20" s="44">
         <v>5.4</v>
       </c>
-      <c r="H20" s="83">
+      <c r="H20" s="77">
         <v>7.6</v>
       </c>
       <c r="I20" s="44">
         <v>6.1</v>
       </c>
-      <c r="J20" s="83">
+      <c r="J20" s="77">
         <v>5.0999999999999996</v>
       </c>
-      <c r="K20" s="88">
+      <c r="K20" s="82">
         <v>6.9</v>
       </c>
     </row>
@@ -7986,7 +7986,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8009,24 +8009,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8036,29 +8036,29 @@
       <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
       <c r="I3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="60" t="s">
+      <c r="K3" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="61"/>
-      <c r="M3" s="60" t="s">
+      <c r="L3" s="87"/>
+      <c r="M3" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="61"/>
-      <c r="O3" s="60" t="s">
+      <c r="N3" s="87"/>
+      <c r="O3" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="62"/>
+      <c r="P3" s="88"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -9124,7 +9124,7 @@
   <dimension ref="A1:S53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9149,61 +9149,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="60" t="s">
+      <c r="E3" s="87"/>
+      <c r="F3" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="60" t="s">
+      <c r="G3" s="87"/>
+      <c r="H3" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="61"/>
-      <c r="J3" s="60" t="s">
+      <c r="I3" s="87"/>
+      <c r="J3" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="61"/>
-      <c r="L3" s="60" t="s">
+      <c r="K3" s="87"/>
+      <c r="L3" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="61"/>
-      <c r="N3" s="60" t="s">
+      <c r="M3" s="87"/>
+      <c r="N3" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="61"/>
-      <c r="P3" s="60" t="s">
+      <c r="O3" s="87"/>
+      <c r="P3" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="60" t="s">
+      <c r="Q3" s="87"/>
+      <c r="R3" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="62"/>
+      <c r="S3" s="88"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -9277,51 +9277,35 @@
       <c r="D5" s="28">
         <v>1.5625E-2</v>
       </c>
-      <c r="E5" s="27">
-        <v>1024.001</v>
-      </c>
+      <c r="E5" s="27"/>
       <c r="F5" s="28">
         <v>0.25</v>
       </c>
-      <c r="G5" s="27">
-        <v>1024.001</v>
-      </c>
+      <c r="G5" s="27"/>
       <c r="H5" s="28">
         <v>7.8125E-3</v>
       </c>
-      <c r="I5" s="27">
-        <v>1024.001</v>
-      </c>
+      <c r="I5" s="27"/>
       <c r="J5" s="57">
         <v>0.25</v>
       </c>
-      <c r="K5" s="27">
-        <v>1024.001</v>
-      </c>
+      <c r="K5" s="27"/>
       <c r="L5" s="12">
         <v>3.90625E-3</v>
       </c>
-      <c r="M5" s="27">
-        <v>1024.001</v>
-      </c>
+      <c r="M5" s="27"/>
       <c r="N5" s="27">
         <v>-1024</v>
       </c>
-      <c r="O5" s="27">
-        <v>1024.001</v>
-      </c>
+      <c r="O5" s="27"/>
       <c r="P5" s="28">
         <v>6.25E-2</v>
       </c>
-      <c r="Q5" s="27">
-        <v>1024.001</v>
-      </c>
+      <c r="Q5" s="27"/>
       <c r="R5" s="28">
         <v>7.8125E-3</v>
       </c>
-      <c r="S5" s="27">
-        <v>1024.001</v>
-      </c>
+      <c r="S5" s="27"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -9331,51 +9315,35 @@
       <c r="D6" s="31">
         <v>7.8125E-3</v>
       </c>
-      <c r="E6" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="E6" s="29"/>
       <c r="F6" s="31">
         <v>1.953125E-3</v>
       </c>
-      <c r="G6" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="G6" s="29"/>
       <c r="H6" s="30">
         <v>7.8125E-3</v>
       </c>
-      <c r="I6" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="I6" s="29"/>
       <c r="J6" s="30">
         <v>0.25</v>
       </c>
-      <c r="K6" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="K6" s="29"/>
       <c r="L6" s="30">
         <v>0.125</v>
       </c>
-      <c r="M6" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="M6" s="29"/>
       <c r="N6" s="29">
         <v>-4</v>
       </c>
-      <c r="O6" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="O6" s="29"/>
       <c r="P6" s="31">
         <v>6.25E-2</v>
       </c>
-      <c r="Q6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="R6" s="29">
+      <c r="Q6" s="29"/>
+      <c r="R6" s="13">
         <v>0.125</v>
       </c>
-      <c r="S6" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="S6" s="29"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -9388,51 +9356,35 @@
       <c r="D7" s="31">
         <v>1.5625E-2</v>
       </c>
-      <c r="E7" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="E7" s="29"/>
       <c r="F7" s="31">
         <v>7.8125E-3</v>
       </c>
-      <c r="G7" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="G7" s="29"/>
       <c r="H7" s="29">
         <v>32</v>
       </c>
-      <c r="I7" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="I7" s="29"/>
       <c r="J7" s="30">
         <v>0.5</v>
       </c>
-      <c r="K7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="L7" s="29">
+      <c r="K7" s="29"/>
+      <c r="L7" s="13">
         <v>1.953125E-3</v>
       </c>
-      <c r="M7" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="M7" s="29"/>
       <c r="N7" s="31">
         <v>-9.765625E-4</v>
       </c>
-      <c r="O7" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="O7" s="29"/>
       <c r="P7" s="30">
         <v>0.25</v>
       </c>
-      <c r="Q7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="R7" s="30">
+      <c r="Q7" s="29"/>
+      <c r="R7" s="13">
         <v>1.953125E-3</v>
       </c>
-      <c r="S7" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="S7" s="29"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
@@ -9443,51 +9395,35 @@
       <c r="D8" s="29">
         <v>2</v>
       </c>
-      <c r="E8" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="E8" s="29"/>
       <c r="F8" s="30">
         <v>6.25E-2</v>
       </c>
-      <c r="G8" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="G8" s="29"/>
       <c r="H8" s="31">
         <v>0.125</v>
       </c>
-      <c r="I8" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="I8" s="29"/>
       <c r="J8" s="19">
         <v>0.5</v>
       </c>
-      <c r="K8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="L8" s="19">
+      <c r="K8" s="29"/>
+      <c r="L8" s="31">
         <v>3.125E-2</v>
       </c>
-      <c r="M8" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="M8" s="29"/>
       <c r="N8" s="13">
         <v>-9.765625E-4</v>
       </c>
-      <c r="O8" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="O8" s="29"/>
       <c r="P8" s="13">
         <v>0.125</v>
       </c>
-      <c r="Q8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="R8" s="29">
+      <c r="Q8" s="29"/>
+      <c r="R8" s="13">
         <v>3.90625E-3</v>
       </c>
-      <c r="S8" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="S8" s="29"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -9502,51 +9438,35 @@
       <c r="D9" s="30">
         <v>0.2</v>
       </c>
-      <c r="E9" s="29">
-        <v>1</v>
-      </c>
+      <c r="E9" s="29"/>
       <c r="F9" s="19">
         <v>0.6</v>
       </c>
-      <c r="G9" s="29">
-        <v>1</v>
-      </c>
+      <c r="G9" s="29"/>
       <c r="H9" s="30">
         <v>0.8</v>
       </c>
-      <c r="I9" s="29">
-        <v>1</v>
-      </c>
-      <c r="J9" s="30">
+      <c r="I9" s="29"/>
+      <c r="J9" s="13">
         <v>1E-3</v>
       </c>
-      <c r="K9" s="29">
-        <v>1</v>
-      </c>
-      <c r="L9" s="19">
+      <c r="K9" s="29"/>
+      <c r="L9" s="13">
         <v>1E-3</v>
       </c>
-      <c r="M9" s="29">
-        <v>1</v>
-      </c>
+      <c r="M9" s="29"/>
       <c r="N9" s="19">
         <v>0.7</v>
       </c>
-      <c r="O9" s="29">
-        <v>1</v>
-      </c>
+      <c r="O9" s="29"/>
       <c r="P9" s="30">
         <v>0.6</v>
       </c>
-      <c r="Q9" s="29">
-        <v>1</v>
-      </c>
+      <c r="Q9" s="29"/>
       <c r="R9" s="19">
         <v>0.8</v>
       </c>
-      <c r="S9" s="29">
-        <v>1</v>
-      </c>
+      <c r="S9" s="29"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -9556,51 +9476,35 @@
       <c r="D10" s="30">
         <v>0.999</v>
       </c>
-      <c r="E10" s="29">
-        <v>1</v>
-      </c>
+      <c r="E10" s="29"/>
       <c r="F10" s="19">
         <v>0.3</v>
       </c>
-      <c r="G10" s="29">
-        <v>1</v>
-      </c>
+      <c r="G10" s="29"/>
       <c r="H10" s="30">
         <v>0.7</v>
       </c>
-      <c r="I10" s="29">
-        <v>1</v>
-      </c>
-      <c r="J10" s="19">
+      <c r="I10" s="29"/>
+      <c r="J10" s="13">
         <v>1E-3</v>
       </c>
-      <c r="K10" s="29">
-        <v>1</v>
-      </c>
+      <c r="K10" s="29"/>
       <c r="L10" s="29">
         <v>0.999</v>
       </c>
-      <c r="M10" s="29">
-        <v>1</v>
-      </c>
+      <c r="M10" s="29"/>
       <c r="N10" s="30">
         <v>0.01</v>
       </c>
-      <c r="O10" s="29">
-        <v>1</v>
-      </c>
+      <c r="O10" s="29"/>
       <c r="P10" s="30">
         <v>0.99</v>
       </c>
-      <c r="Q10" s="29">
-        <v>1</v>
-      </c>
+      <c r="Q10" s="29"/>
       <c r="R10" s="19">
         <v>0.1</v>
       </c>
-      <c r="S10" s="29">
-        <v>1</v>
-      </c>
+      <c r="S10" s="29"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -9613,51 +9517,35 @@
       <c r="D11" s="30">
         <v>0.4</v>
       </c>
-      <c r="E11" s="29">
-        <v>1</v>
-      </c>
+      <c r="E11" s="29"/>
       <c r="F11" s="30">
         <v>0.6</v>
       </c>
-      <c r="G11" s="29">
-        <v>1</v>
-      </c>
+      <c r="G11" s="29"/>
       <c r="H11" s="30">
         <v>0.8</v>
       </c>
-      <c r="I11" s="29">
-        <v>1</v>
-      </c>
+      <c r="I11" s="29"/>
       <c r="J11" s="30">
         <v>0.1</v>
       </c>
-      <c r="K11" s="29">
-        <v>1</v>
-      </c>
+      <c r="K11" s="29"/>
       <c r="L11" s="30">
         <v>0.3</v>
       </c>
-      <c r="M11" s="29">
-        <v>1</v>
-      </c>
+      <c r="M11" s="29"/>
       <c r="N11" s="19">
         <v>0.7</v>
       </c>
-      <c r="O11" s="29">
-        <v>1</v>
-      </c>
+      <c r="O11" s="29"/>
       <c r="P11" s="30">
         <v>0.7</v>
       </c>
-      <c r="Q11" s="29">
-        <v>1</v>
-      </c>
+      <c r="Q11" s="29"/>
       <c r="R11" s="19">
         <v>0.4</v>
       </c>
-      <c r="S11" s="29">
-        <v>1</v>
-      </c>
+      <c r="S11" s="29"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -9668,51 +9556,35 @@
       <c r="D12" s="30">
         <v>0.4</v>
       </c>
-      <c r="E12" s="29">
-        <v>1</v>
-      </c>
+      <c r="E12" s="29"/>
       <c r="F12" s="30">
         <v>0.7</v>
       </c>
-      <c r="G12" s="29">
-        <v>1</v>
-      </c>
+      <c r="G12" s="29"/>
       <c r="H12" s="30">
         <v>0.9</v>
       </c>
-      <c r="I12" s="29">
-        <v>1</v>
-      </c>
+      <c r="I12" s="29"/>
       <c r="J12" s="19">
         <v>0.9</v>
       </c>
-      <c r="K12" s="29">
-        <v>1</v>
-      </c>
+      <c r="K12" s="29"/>
       <c r="L12" s="30">
         <v>0.01</v>
       </c>
-      <c r="M12" s="29">
-        <v>1</v>
-      </c>
-      <c r="N12" s="19">
+      <c r="M12" s="29"/>
+      <c r="N12" s="30">
         <v>0.01</v>
       </c>
-      <c r="O12" s="29">
-        <v>1</v>
-      </c>
+      <c r="O12" s="29"/>
       <c r="P12" s="30">
         <v>0.1</v>
       </c>
-      <c r="Q12" s="29">
-        <v>1</v>
-      </c>
+      <c r="Q12" s="29"/>
       <c r="R12" s="31">
         <v>1E-3</v>
       </c>
-      <c r="S12" s="29">
-        <v>1</v>
-      </c>
+      <c r="S12" s="29"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -9917,7 +9789,7 @@
       <c r="L16" s="31">
         <v>1.5625E-2</v>
       </c>
-      <c r="M16" s="29">
+      <c r="M16" s="30">
         <v>0.2509765625</v>
       </c>
       <c r="N16" s="29">
@@ -10009,10 +9881,10 @@
       <c r="E18" s="29">
         <v>128.0009765625</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="29">
         <v>32</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="29">
         <v>1024.0009765625</v>
       </c>
       <c r="H18" s="31">

</xml_diff>